<commit_message>
Changed the way the timestep is extracted from an input spreadsheet (using the max number of times each year is repeated on row 11)
</commit_message>
<xml_diff>
--- a/data/reg_input/Quarterly Road Data.xlsx
+++ b/data/reg_input/Quarterly Road Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fidias\Coding-related\Python\Traffic-Regression-Tool\data\reg_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6C256F-478B-4145-A2D3-DC4839BA370C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE72231-44E9-453E-B278-48AE10B7A2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10810" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="77">
   <si>
     <t>Confidential</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>pct_val_or_dummy</t>
-  </si>
-  <si>
-    <t>Timestep</t>
-  </si>
-  <si>
-    <t>Quarterly</t>
   </si>
   <si>
     <t>Q2 Seasonality</t>
@@ -1292,23 +1286,23 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BO50"/>
+  <dimension ref="B2:BO40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="G47" sqref="G47:I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="3" width="9.09765625" customWidth="1"/>
-    <col min="4" max="4" width="19.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="9.09765625" customWidth="1"/>
-    <col min="10" max="10" width="7.796875" customWidth="1"/>
-    <col min="11" max="19" width="9.09765625" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="19" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1378,7 +1372,7 @@
       <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
     </row>
-    <row r="3" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1448,7 +1442,7 @@
       <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
     </row>
-    <row r="4" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1512,7 @@
       <c r="BN4" s="1"/>
       <c r="BO4" s="1"/>
     </row>
-    <row r="6" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1588,7 +1582,7 @@
       <c r="BN6" s="1"/>
       <c r="BO6" s="1"/>
     </row>
-    <row r="11" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:67" x14ac:dyDescent="0.2">
       <c r="G11" s="6">
         <v>2012</v>
       </c>
@@ -1734,7 +1728,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="12" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:67" x14ac:dyDescent="0.2">
       <c r="D12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>4</v>
@@ -1881,7 +1875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:67" x14ac:dyDescent="0.2">
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2033,7 +2027,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:67" x14ac:dyDescent="0.2">
       <c r="D14" s="3" t="s">
         <v>58</v>
       </c>
@@ -2185,7 +2179,7 @@
         <v>10384.764243798347</v>
       </c>
     </row>
-    <row r="15" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:67" x14ac:dyDescent="0.2">
       <c r="D15" s="8" t="s">
         <v>60</v>
       </c>
@@ -2337,7 +2331,7 @@
         <v>13821.96612539767</v>
       </c>
     </row>
-    <row r="16" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:67" x14ac:dyDescent="0.2">
       <c r="D16" s="8" t="s">
         <v>61</v>
       </c>
@@ -2489,7 +2483,7 @@
         <v>6023.4282608695648</v>
       </c>
     </row>
-    <row r="17" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D17" s="8" t="s">
         <v>62</v>
       </c>
@@ -2641,7 +2635,7 @@
         <v>725.64086423046149</v>
       </c>
     </row>
-    <row r="18" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D18" s="8" t="s">
         <v>63</v>
       </c>
@@ -2793,7 +2787,7 @@
         <v>1828.6284199363733</v>
       </c>
     </row>
-    <row r="19" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D19" s="8" t="s">
         <v>64</v>
       </c>
@@ -2945,7 +2939,7 @@
         <v>284.40869565217389</v>
       </c>
     </row>
-    <row r="22" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:54" x14ac:dyDescent="0.2">
       <c r="G22" s="6">
         <v>2012</v>
       </c>
@@ -3091,7 +3085,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="23" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:54" x14ac:dyDescent="0.2">
       <c r="G23" s="6" t="s">
         <v>4</v>
       </c>
@@ -3237,7 +3231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D24" s="7" t="s">
         <v>65</v>
       </c>
@@ -3389,7 +3383,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D25" s="8" t="s">
         <v>66</v>
       </c>
@@ -3541,7 +3535,7 @@
         <v>54242.462800000001</v>
       </c>
     </row>
-    <row r="26" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
         <v>67</v>
       </c>
@@ -3693,7 +3687,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="27" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
         <v>68</v>
       </c>
@@ -3845,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="s">
         <v>69</v>
       </c>
@@ -3997,7 +3991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
         <v>70</v>
       </c>
@@ -4149,7 +4143,7 @@
         <v>111.08489131012149</v>
       </c>
     </row>
-    <row r="30" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="s">
         <v>71</v>
       </c>
@@ -4301,9 +4295,9 @@
         <v>148.21550411007593</v>
       </c>
     </row>
-    <row r="31" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D31" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>73</v>
@@ -4497,9 +4491,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:54" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:54" x14ac:dyDescent="0.2">
       <c r="D32" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>73</v>
@@ -4693,9 +4687,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:67" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:67" x14ac:dyDescent="0.2">
       <c r="D33" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>73</v>
@@ -4889,8 +4883,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:67" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:67" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>72</v>
       </c>
@@ -4960,14 +4954,6 @@
       <c r="BN40" s="1"/>
       <c r="BO40" s="1"/>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G50" t="s">
-        <v>74</v>
-      </c>
-      <c r="H50" t="s">
-        <v>75</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H50" xr:uid="{4D480346-D891-4739-8DAD-77B94267578F}">

</xml_diff>